<commit_message>
bug no back msm
</commit_message>
<xml_diff>
--- a/DotNetExcel/StarkBankExcel/StarkBank.xlsx
+++ b/DotNetExcel/StarkBankExcel/StarkBank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stark - Admin\Documents\deploy-cartshop-hoje\sdk-excel\DotNetExcel\StarkBankExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B759197-E2E7-41B4-962B-ABC3A6720429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF3CF4F-E6B8-46AD-9AFD-A5598032F1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="2" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
   </bookViews>
@@ -753,23 +753,6 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6BFC21A776750A64A676B05D6ACABCB02B86D6"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="5974E136658C5454320585C85BAB48B9439E65"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -782,7 +765,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -799,7 +782,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -816,7 +799,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -833,7 +816,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -846,6 +829,23 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX19.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5FE4E9EDE5117D54C395AB0B52D849B4179075"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -872,23 +872,6 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5FE4E9EDE5117D54C395AB0B52D849B4179075"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX21.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="690DE6C82662BD648A469A3C645736EF297746"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -901,7 +884,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX21.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -918,7 +901,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX22.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -935,7 +918,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX23.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -952,7 +935,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -969,7 +952,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -986,7 +969,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1003,7 +986,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1020,12 +1003,29 @@
 </ax:ocx>
 </file>
 
+<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="21156A5D42671D24110290D22610E26CEF0122"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
 <file path=xl/activeX/activeX29.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="21156A5D42671D24110290D22610E26CEF0122"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="36BF4D76D36CAA346A9392633D35C8E7F4F293"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1059,7 +1059,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="36BF4D76D36CAA346A9392633D35C8E7F4F293"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4BDD5BFBC494C944E75484BA43B9AFC575EDE4"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1076,23 +1076,6 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4BDD5BFBC494C944E75484BA43B9AFC575EDE4"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX32.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="544CE9B5B5F4C8548335AFF35313355602FAD5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -1105,7 +1088,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX32.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1122,7 +1105,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1139,7 +1122,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1156,7 +1139,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1173,7 +1156,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1190,7 +1173,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1207,12 +1190,29 @@
 </ax:ocx>
 </file>
 
+<file path=xl/activeX/activeX38.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2F27997732C2CB2441C298BB24A21C18565F42"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
 <file path=xl/activeX/activeX39.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2F27997732C2CB2441C298BB24A21C18565F42"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="32D5429B8373DD34ED03A9043941F439C19723"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1246,7 +1246,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="32D5429B8373DD34ED03A9043941F439C19723"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4725C0A2E4AB894430D4AEF74EE21D1AD6A734"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1263,7 +1263,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4725C0A2E4AB894430D4AEF74EE21D1AD6A734"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5F3C3A5AA5DBB654AFD5A7C25896612CBE6DC5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1280,23 +1280,6 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5F3C3A5AA5DBB654AFD5A7C25896612CBE6DC5"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX43.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="6D5513A176D11B6489268BF06C26AC9C7986A6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -1309,7 +1292,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX43.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1326,7 +1309,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX44.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1343,7 +1326,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX45.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1360,7 +1343,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX46.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1377,7 +1360,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX47.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1394,12 +1377,29 @@
 </ax:ocx>
 </file>
 
+<file path=xl/activeX/activeX48.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4EDC5AE2D4725F442D54BDB348E5FBB86B52C4"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
 <file path=xl/activeX/activeX49.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4EDC5AE2D4725F442D54BDB348E5FBB86B52C4"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3443F6D933A917348513994830A35447867593"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1433,23 +1433,6 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3443F6D933A917348513994830A35447867593"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX51.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="2F31A0EA52B80A243F02887A226A80BA2346A2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -1462,7 +1445,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX51.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1479,7 +1462,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX52.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1496,7 +1479,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX53.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1513,7 +1496,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX54.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1530,7 +1513,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX55.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1547,7 +1530,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX56.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1564,7 +1547,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX57.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1581,7 +1564,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX58.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1594,6 +1577,23 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX59.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="209AD430929B0C246352BB46205966BBA32BE2"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1620,23 +1620,6 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="209AD430929B0C246352BB46205966BBA32BE2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX61.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="340115F7C331F8342C23902032B2E1FE922923"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -1649,7 +1632,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX61.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1666,7 +1649,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX62.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1683,7 +1666,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX63.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1700,7 +1683,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX64.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1717,7 +1700,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX65.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1734,7 +1717,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX66.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1751,7 +1734,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX67.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1768,12 +1751,29 @@
 </ax:ocx>
 </file>
 
+<file path=xl/activeX/activeX68.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="42576A9D548EA54490F4BA2045852D9EEA0264"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
 <file path=xl/activeX/activeX69.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="42576A9D548EA54490F4BA2045852D9EEA0264"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="32381B0E43363B340003842439CB6D4833D8F3"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1807,7 +1807,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="32381B0E43363B340003842439CB6D4833D8F3"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="207D2713820AB8246622A7CD26A57A9DCA2162"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1824,7 +1824,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="207D2713820AB8246622A7CD26A57A9DCA2162"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19726D3BD1AD01142191B2C41B5B2D13E650B1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1841,23 +1841,6 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19726D3BD1AD01142191B2C41B5B2D13E650B1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX73.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="1B7A977A61ADF41453E1BBBE1183429619DB11"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -1870,7 +1853,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX73.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1887,7 +1870,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX74.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1904,7 +1887,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX75.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1921,7 +1904,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX76.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1938,7 +1921,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX77.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1955,7 +1938,7 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX79.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX78.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1967,6 +1950,23 @@
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="3149"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX79.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="33A9EADB835964348083B921335A9469D78A13"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -1994,7 +1994,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="33A9EADB835964348083B921335A9469D78A13"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="245B62680258F8244B928BF02F0D73C394B3A2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2011,7 +2011,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="245B62680258F8244B928BF02F0D73C394B3A2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="632A921A961CC6648D5697386AA1DF460A0236"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2028,7 +2028,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="632A921A961CC6648D5697386AA1DF460A0236"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="482B56B2D4F09144EA9495AD4E1391B3ADA544"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2045,7 +2045,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="482B56B2D4F09144EA9495AD4E1391B3ADA544"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3C148BBC83328034CB4383F53575DFC2E2D673"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2062,7 +2062,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3C148BBC83328034CB4383F53575DFC2E2D673"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2DE4C20F929D4D245012850329872D57BE1542"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2079,7 +2079,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2DE4C20F929D4D245012850329872D57BE1542"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1441CBD291E7921466418469122C7CFF2CD931"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2096,7 +2096,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1441CBD291E7921466418469122C7CFF2CD931"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="676BBF00A6812B64BBB6BA716DB953807A8EA6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2113,23 +2113,6 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="676BBF00A6812B64BBB6BA716DB953807A8EA6"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX88.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
   <ax:ocxPr ax:name="Cookie" ax:value="560AC6FB15F17754F6558A0F58035E0AF7ED85"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
@@ -2142,12 +2125,29 @@
 </ax:ocx>
 </file>
 
+<file path=xl/activeX/activeX88.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="423CD9C0343555445FB48C9D4CF7D65D1F3284"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
 <file path=xl/activeX/activeX89.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="423CD9C0343555445FB48C9D4CF7D65D1F3284"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3980FC20730620345FE3A45431A52DCB072F13"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2181,7 +2181,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3980FC20730620345FE3A45431A52DCB072F13"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2596667A2285C4241122B3CF25CD7B218043C2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2194,23 +2194,6 @@
 </file>
 
 <file path=xl/activeX/activeX91.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2596667A2285C4241122B3CF25CD7B218043C2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX92.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -5770,68 +5753,6 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005740100}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>390525</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>390525</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="95238" name="_ActiveXWrapper5" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s95238"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{327028B7-7221-072C-4E2C-E2723D880DA8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11252,7 +11173,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11423,33 +11344,8 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="95238" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="95237" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>390525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>390525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="95238" r:id="rId4" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="95237" r:id="rId6" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
@@ -11468,13 +11364,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="95237" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="95237" r:id="rId4" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="95235" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="95235" r:id="rId6" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -11493,13 +11389,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="95235" r:id="rId8" name="_ActiveXWrapper3"/>
+        <control shapeId="95235" r:id="rId6" name="_ActiveXWrapper3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="95234" r:id="rId10" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+        <control shapeId="95234" r:id="rId8" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -11518,13 +11414,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="95234" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="95234" r:id="rId8" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="95233" r:id="rId12" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="95233" r:id="rId10" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -11543,7 +11439,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="95233" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="95233" r:id="rId10" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Add dynamic size scale
</commit_message>
<xml_diff>
--- a/DotNetExcel/StarkBankExcel/StarkBank.xlsx
+++ b/DotNetExcel/StarkBankExcel/StarkBank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stark - Admin\Documents\deploy-cartshop-hoje\sdk-excel\DotNetExcel\StarkBankExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCED1937-037A-48EB-82E5-F4B10E882AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF6B7AD-546C-4AA4-B22B-B8FCE1ACF816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="1" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="1" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="2" state="hidden" r:id="rId1"/>
@@ -399,7 +399,7 @@
     <t>Ex: 20018-183</t>
   </si>
   <si>
-    <t>Stark Bank SDK Excel Debug - v3.1.1</t>
+    <t>Stark Bank SDK Excel Debug 2 - v3.1.1</t>
   </si>
 </sst>
 </file>
@@ -668,7 +668,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="28A34ED1D2633F2429D291182761C070389522"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="23A4525A1295E524FB7284BA2EA2DC8317EF42"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -685,24 +685,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1626B229C1652514446181B314A00A77AF6681"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1F70BF05619C7F14D001A2031EA2288CEEF621"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="17053D61D1F15A1482019B2C1A4E6D57E3A971"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -714,12 +697,29 @@
 </ax:ocx>
 </file>
 
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19A5453E610F18142DA1BAA91D29A587ED2E11"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4313"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
 <file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="23FDAD7A329F60245422A56B22EA1482F84402"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D58F8DCE161321493A19D8C10118F3363B411"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -736,7 +736,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2EF132486228D8243F428A6C298561D10E6622"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="10F831FB013D30140151820D1AB0BB140FD961"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -753,7 +753,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="23A4525A1295E524FB7284BA2EA2DC8317EF42"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="28A34ED1D2633F2429D291182761C070389522"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -770,19 +770,36 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5974E136658C5454320585C85BAB48B9439E65"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="15BA0FB321DE6D148D81BF60113447A8E50371"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2AE3450482C58E244C5291B3282A90F9A78E42"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -799,36 +816,19 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2AE3450482C58E244C5291B3282A90F9A78E42"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5974E136658C5454320585C85BAB48B9439E65"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="15BA0FB321DE6D148D81BF60113447A8E50371"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -838,14 +838,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="43935BDA7439194471449D234CFD527D9886B4"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="80815DC5B82C3B8498489E26894C5C52875E28"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1588"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -855,7 +855,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="10F831FB013D30140151820D1AB0BB140FD961"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2EF132486228D8243F428A6C298561D10E6622"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -872,14 +872,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5FE4E9EDE5117D54C395AB0B52D849B4179075"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="71F4FF3617034374D487A4537B51302A0C89B7"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -906,14 +906,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="71F4FF3617034374D487A4537B51302A0C89B7"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5FE4E9EDE5117D54C395AB0B52D849B4179075"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -923,19 +923,70 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="80815DC5B82C3B8498489E26894C5C52875E28"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="43935BDA7439194471449D234CFD527D9886B4"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1588"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6D72D142762FA7648186B99160B384DA4EEAD6"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="576D85FB2525B8547055A14351ED593B73E215"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4DD8155564BBBB442F449A794155F293DF1F94"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -952,12 +1003,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4DD8155564BBBB442F449A794155F293DF1F94"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4BDD5BFBC494C944E75484BA43B9AFC575EDE4"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -969,29 +1020,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX29.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="576D85FB2525B8547055A14351ED593B73E215"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6D72D142762FA7648186B99160B384DA4EEAD6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="36BF4D76D36CAA346A9392633D35C8E7F4F293"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1003,7 +1037,41 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="23FDAD7A329F60245422A56B22EA1482F84402"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX30.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="21156A5D42671D24110290D22610E26CEF0122"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX31.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1020,75 +1088,92 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX32.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="21156A5D42671D24110290D22610E26CEF0122"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="7C9BBDE4E751B574F557BC077FC280926F0487"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D58F8DCE161321493A19D8C10118F3363B411"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6EAFFE9C06D4276431A6BB2F6072D3CF2C1786"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="36BF4D76D36CAA346A9392633D35C8E7F4F293"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1BF3F766D1EC8E14D641AB8818D8695A960D41"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4BDD5BFBC494C944E75484BA43B9AFC575EDE4"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="29E4B6D5F2B5EF24B732AC612476A095FC12F2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3AA2985733B4083434D3B3DA395B83B5AB5FB3"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1105,97 +1190,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3AA2985733B4083434D3B3DA395B83B5AB5FB3"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="29E4B6D5F2B5EF24B732AC612476A095FC12F2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1BF3F766D1EC8E14D641AB8818D8695A960D41"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6EAFFE9C06D4276431A6BB2F6072D3CF2C1786"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="7C9BBDE4E751B574F557BC077FC280926F0487"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX38.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D3C8440119274147F5190E81CB29314F1A0B1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5F3C3A5AA5DBB654AFD5A7C25896612CBE6DC5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1212,7 +1212,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2F27997732C2CB2441C298BB24A21C18565F42"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4725C0A2E4AB894430D4AEF74EE21D1AD6A734"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1229,13 +1229,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19A5453E610F18142DA1BAA91D29A587ED2E11"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1F70BF05619C7F14D001A2031EA2288CEEF621"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4313"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -1263,7 +1263,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4725C0A2E4AB894430D4AEF74EE21D1AD6A734"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2F27997732C2CB2441C298BB24A21C18565F42"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1280,7 +1280,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5F3C3A5AA5DBB654AFD5A7C25896612CBE6DC5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D3C8440119274147F5190E81CB29314F1A0B1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1297,19 +1297,36 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6D5513A176D11B6489268BF06C26AC9C7986A6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="9C5D0F81D9A7DC9451D986E29349E294E0E0F9"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX44.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="8A681C04683975842508B2258073BEA1C60FD8"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX45.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1326,41 +1343,126 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX46.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="8A681C04683975842508B2258073BEA1C60FD8"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6D5513A176D11B6489268BF06C26AC9C7986A6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX47.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="9C5D0F81D9A7DC9451D986E29349E294E0E0F9"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="190EB7A1C18BFD142EB1A75D1D8ECE9AC6A921"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3096"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX48.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2F31A0EA52B80A243F02887A226A80BA2346A2"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3334"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1217"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX49.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3443F6D933A917348513994830A35447867593"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1626B229C1652514446181B314A00A77AF6681"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4EDC5AE2D4725F442D54BDB348E5FBB86B52C4"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX51.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="581AFF66D5395E54CBC5BEBA52A895EF8D96F5"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX52.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1377,12 +1479,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX53.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="581AFF66D5395E54CBC5BEBA52A895EF8D96F5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="64B7B760262CDD643836A79A641DDB36424F16"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1394,12 +1496,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX54.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4EDC5AE2D4725F442D54BDB348E5FBB86B52C4"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="192AED9321906F1430518AA91C61F691A49AE1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1411,29 +1513,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX55.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="17053D61D1F15A1482019B2C1A4E6D57E3A971"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3443F6D933A917348513994830A35447867593"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2FAFF23AA2246924D782B58F21CB01DE2B8C82"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1445,41 +1530,41 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX56.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2F31A0EA52B80A243F02887A226A80BA2346A2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="393B0D4DB376B1348C53AA283ED005A8E39383"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3334"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1217"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX57.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="190EB7A1C18BFD142EB1A75D1D8ECE9AC6A921"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="43443F65340DC5448034B84249A78BF6899C14"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3096"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX58.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1496,92 +1581,75 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX59.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="43443F65340DC5448034B84249A78BF6899C14"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="41CF79F694E72D449634A36244C31DA4F7C064"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="393B0D4DB376B1348C53AA283ED005A8E39383"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1DB344D2F14249140061BD5D11E614111405C1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4392"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX60.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2FAFF23AA2246924D782B58F21CB01DE2B8C82"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="340115F7C331F8342C23902032B2E1FE922923"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX61.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="192AED9321906F1430518AA91C61F691A49AE1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="209AD430929B0C246352BB46205966BBA32BE2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX58.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="64B7B760262CDD643836A79A641DDB36424F16"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX62.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1598,80 +1666,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D1500907189BD14DA51B2181B162FBD75FE31"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX60.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="209AD430929B0C246352BB46205966BBA32BE2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX61.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="340115F7C331F8342C23902032B2E1FE922923"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX62.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="41CF79F694E72D449634A36244C31DA4F7C064"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX63.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1FF48C76A17A8C14A1D1B461189CB6BA129791"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5FCC13B9257A75548E65A9E458AA0E6A413BF5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1688,7 +1688,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="23587ECD629DA1245032AC232F0D6B45106E92"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4F2081B3648833443864BB8143FD2C02F9E634"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1722,7 +1722,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4F2081B3648833443864BB8143FD2C02F9E634"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="23587ECD629DA1245032AC232F0D6B45106E92"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1739,7 +1739,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5FCC13B9257A75548E65A9E458AA0E6A413BF5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1FF48C76A17A8C14A1D1B461189CB6BA129791"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1756,7 +1756,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5B4A34D975B853543985A7E75523690B60EC35"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19726D3BD1AD01142191B2C41B5B2D13E650B1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1773,7 +1773,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="42576A9D548EA54490F4BA2045852D9EEA0264"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="207D2713820AB8246622A7CD26A57A9DCA2162"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1790,14 +1790,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1BD6BA4211BC3E14DAF185961A2B376D133421"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1CC3318201EE2A1421C19CEB15987574AED511"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1824,7 +1824,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="207D2713820AB8246622A7CD26A57A9DCA2162"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="42576A9D548EA54490F4BA2045852D9EEA0264"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1841,7 +1841,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19726D3BD1AD01142191B2C41B5B2D13E650B1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5B4A34D975B853543985A7E75523690B60EC35"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1858,14 +1858,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1B7A977A61ADF41453E1BBBE1183429619DB11"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="51A95A66553942547D759A7153A00908FCA885"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3281"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1875,7 +1875,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="232EEE2C927B21244D728DA228DC1AAB22C9E2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4E23FE0EC4C93C4470948DA849AEEC73F9C744"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1909,7 +1909,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4E23FE0EC4C93C4470948DA849AEEC73F9C744"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="232EEE2C927B21244D728DA228DC1AAB22C9E2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1926,14 +1926,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="51A95A66553942547D759A7153A00908FCA885"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1B7A977A61ADF41453E1BBBE1183429619DB11"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3281"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1943,7 +1943,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5B4126E875ABC55427F5B28E55218522354BA5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="632A921A961CC6648D5697386AA1DF460A0236"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1960,13 +1960,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="43953CE6E45013447B8491244183EC3B869614"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="245B62680258F8244B928BF02F0D73C394B3A2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3149"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -1977,14 +1977,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1CC3318201EE2A1421C19CEB15987574AED511"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1BD6BA4211BC3E14DAF185961A2B376D133421"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2011,13 +2011,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="245B62680258F8244B928BF02F0D73C394B3A2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="43953CE6E45013447B8491244183EC3B869614"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3149"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -2028,7 +2028,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="632A921A961CC6648D5697386AA1DF460A0236"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5B4126E875ABC55427F5B28E55218522354BA5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2045,7 +2045,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="482B56B2D4F09144EA9495AD4E1391B3ADA544"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="676BBF00A6812B64BBB6BA716DB953807A8EA6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2062,7 +2062,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3C148BBC83328034CB4383F53575DFC2E2D673"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1441CBD291E7921466418469122C7CFF2CD931"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2096,7 +2096,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1441CBD291E7921466418469122C7CFF2CD931"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3C148BBC83328034CB4383F53575DFC2E2D673"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2113,7 +2113,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="676BBF00A6812B64BBB6BA716DB953807A8EA6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="482B56B2D4F09144EA9495AD4E1391B3ADA544"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2130,14 +2130,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="560AC6FB15F17754F6558A0F58035E0AF7ED85"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1F6AA8BD81815014DA61A5D71870FA81614161"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1482"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2147,7 +2147,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="423CD9C0343555445FB48C9D4CF7D65D1F3284"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2596667A2285C4241122B3CF25CD7B218043C2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2164,13 +2164,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1DB344D2F14249140061BD5D11E614111405C1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D1500907189BD14DA51B2181B162FBD75FE31"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4392"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -2198,7 +2198,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2596667A2285C4241122B3CF25CD7B218043C2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="423CD9C0343555445FB48C9D4CF7D65D1F3284"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2215,14 +2215,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1F6AA8BD81815014DA61A5D71870FA81614161"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="560AC6FB15F17754F6558A0F58035E0AF7ED85"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1482"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -8403,8 +8403,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3078" r:id="rId4" name="_ActiveXWrapper6">
+        <control shapeId="3073" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>542925</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3073" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3074" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>561975</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3074" r:id="rId6" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3075" r:id="rId8" name="_ActiveXWrapper7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3075" r:id="rId8" name="_ActiveXWrapper7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3076" r:id="rId10" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>723900</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3076" r:id="rId10" name="_ActiveXWrapper8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3077" r:id="rId12" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3077" r:id="rId12" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3078" r:id="rId14" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -8423,132 +8548,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3078" r:id="rId4" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3077" r:id="rId6" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3077" r:id="rId6" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3076" r:id="rId8" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>723900</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3076" r:id="rId8" name="_ActiveXWrapper8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3075" r:id="rId10" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3075" r:id="rId10" name="_ActiveXWrapper7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3074" r:id="rId12" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3074" r:id="rId12" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3073" r:id="rId14" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>542925</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3073" r:id="rId14" name="_ActiveXWrapper1"/>
+        <control shapeId="3078" r:id="rId14" name="_ActiveXWrapper6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8665,8 +8665,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="16389" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="16390" r:id="rId4" name="_ActiveXWrapper6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1209675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>981075</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16390" r:id="rId4" name="_ActiveXWrapper6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16385" r:id="rId6" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1162050</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16385" r:id="rId6" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16386" r:id="rId8" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1162050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16386" r:id="rId8" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16387" r:id="rId10" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1076325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16387" r:id="rId10" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16388" r:id="rId12" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1200150</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>971550</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16388" r:id="rId12" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16389" r:id="rId14" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -8685,132 +8810,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="16389" r:id="rId4" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16388" r:id="rId6" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>971550</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16388" r:id="rId6" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16387" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1076325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16387" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16386" r:id="rId10" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1162050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16386" r:id="rId10" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16385" r:id="rId12" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1162050</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16385" r:id="rId12" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16390" r:id="rId14" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1209675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>981075</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16390" r:id="rId14" name="_ActiveXWrapper6"/>
+        <control shapeId="16389" r:id="rId14" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8917,8 +8917,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="73729" r:id="rId3" name="_ActiveXWrapper1">
+        <control shapeId="73732" r:id="rId3" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>419100</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="73732" r:id="rId3" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="73731" r:id="rId5" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="73731" r:id="rId5" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="73730" r:id="rId7" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>466725</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="73730" r:id="rId7" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="73729" r:id="rId9" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -8937,82 +9012,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="73729" r:id="rId3" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="73730" r:id="rId5" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>466725</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="73730" r:id="rId5" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="73731" r:id="rId7" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="73731" r:id="rId7" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="73732" r:id="rId9" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>419100</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="73732" r:id="rId9" name="_ActiveXWrapper4"/>
+        <control shapeId="73729" r:id="rId9" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9158,52 +9158,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="52225" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="52229" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>1266825</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>1181100</xdr:colOff>
+                <xdr:colOff>2428875</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="52225" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="52229" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="52226" r:id="rId6" name="_ActiveXWrapper2">
+        <control shapeId="52228" r:id="rId6" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>2514600</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1171575</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>723900</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="52226" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="52228" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9233,52 +9233,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="52228" r:id="rId10" name="_ActiveXWrapper4">
+        <control shapeId="52226" r:id="rId10" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>2514600</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>723900</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1171575</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="52228" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="52226" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="52229" r:id="rId12" name="_ActiveXWrapper5">
+        <control shapeId="52225" r:id="rId12" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>1266825</xdr:colOff>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>180975</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>2428875</xdr:colOff>
+                <xdr:colOff>1181100</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="52229" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="52225" r:id="rId12" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9394,52 +9394,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20485" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="20481" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20485" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="20481" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20484" r:id="rId6" name="_ActiveXWrapper4">
+        <control shapeId="20482" r:id="rId6" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>390525</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20484" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="20482" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9469,52 +9469,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20482" r:id="rId10" name="_ActiveXWrapper2">
+        <control shapeId="20484" r:id="rId10" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>390525</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20482" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="20484" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20481" r:id="rId12" name="_ActiveXWrapper1">
+        <control shapeId="20485" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20481" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="20485" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9609,52 +9609,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="8197" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1257300</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="8197" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8194" r:id="rId6" name="_ActiveXWrapper2">
+        <control shapeId="8196" r:id="rId6" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1247775</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8194" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="8196" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9684,52 +9684,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8196" r:id="rId10" name="_ActiveXWrapper4">
+        <control shapeId="8194" r:id="rId10" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1247775</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8196" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="8194" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8197" r:id="rId12" name="_ActiveXWrapper5">
+        <control shapeId="8193" r:id="rId12" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1257300</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8197" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="8193" r:id="rId12" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9826,18 +9826,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="49157" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="49158" r:id="rId4" name="_ActiveXWrapper10">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1485900</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>876300</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>685800</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -9846,32 +9846,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="49157" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="49158" r:id="rId4" name="_ActiveXWrapper10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="49156" r:id="rId6" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
+        <control shapeId="49154" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>942975</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1495425</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>2076450</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>695325</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="49156" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="49154" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9901,43 +9901,43 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="49154" r:id="rId10" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+        <control shapeId="49156" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1495425</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>942975</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>695325</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>2076450</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>95250</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="49154" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="49156" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="49158" r:id="rId12" name="_ActiveXWrapper10">
+        <control shapeId="49157" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>876300</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1485900</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>685800</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -9946,7 +9946,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="49158" r:id="rId12" name="_ActiveXWrapper10"/>
+        <control shapeId="49157" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10062,52 +10062,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24580" r:id="rId4" name="_ActiveXWrapper4">
+        <control shapeId="24582" r:id="rId4" name="_ActiveXWrapper10">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1123950</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1209675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>895350</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>981075</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24580" r:id="rId4" name="_ActiveXWrapper4"/>
+        <control shapeId="24582" r:id="rId4" name="_ActiveXWrapper10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24579" r:id="rId6" name="_ActiveXWrapper3">
+        <control shapeId="24577" r:id="rId6" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1219200</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>990600</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1047750</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24579" r:id="rId6" name="_ActiveXWrapper3"/>
+        <control shapeId="24577" r:id="rId6" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10137,52 +10137,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24577" r:id="rId10" name="_ActiveXWrapper1">
+        <control shapeId="24579" r:id="rId10" name="_ActiveXWrapper3">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1219200</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1047750</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>990600</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24577" r:id="rId10" name="_ActiveXWrapper1"/>
+        <control shapeId="24579" r:id="rId10" name="_ActiveXWrapper3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24582" r:id="rId12" name="_ActiveXWrapper10">
+        <control shapeId="24580" r:id="rId12" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1209675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1123950</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>981075</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>895350</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24582" r:id="rId12" name="_ActiveXWrapper10"/>
+        <control shapeId="24580" r:id="rId12" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10267,52 +10267,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6149" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="6145" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>1333500</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>47625</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>1114425</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1152525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6149" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="6145" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6148" r:id="rId6" name="_ActiveXWrapper4">
+        <control shapeId="6146" r:id="rId6" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>1247775</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>1028700</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1171575</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6148" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="6146" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10342,52 +10342,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6146" r:id="rId10" name="_ActiveXWrapper2">
+        <control shapeId="6148" r:id="rId10" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1247775</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1171575</xdr:colOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>1028700</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>123825</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6146" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="6148" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6145" r:id="rId12" name="_ActiveXWrapper1">
+        <control shapeId="6149" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>1333500</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>47625</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1152525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1114425</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6145" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="6149" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10400,7 +10400,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -10919,8 +10919,333 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1044" r:id="rId4" name="_ActiveXWrapper11">
+        <control shapeId="1047" r:id="rId4" name="_ActiveXWrapper14">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>19</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1047" r:id="rId4" name="_ActiveXWrapper14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1046" r:id="rId6" name="_ActiveXWrapper13">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>19</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1046" r:id="rId6" name="_ActiveXWrapper13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1045" r:id="rId8" name="_ActiveXWrapper12">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>14</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>371475</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1045" r:id="rId8" name="_ActiveXWrapper12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1041" r:id="rId10" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1041" r:id="rId10" name="_ActiveXWrapper8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1040" r:id="rId12" name="_ActiveXWrapper7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1040" r:id="rId12" name="_ActiveXWrapper7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1039" r:id="rId14" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1039" r:id="rId14" name="_ActiveXWrapper6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1038" r:id="rId16" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId16" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1037" r:id="rId18" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>1048575</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1037" r:id="rId18" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1036" r:id="rId20" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>266700</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>1048575</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1036" r:id="rId20" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId22" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>161925</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1035" r:id="rId22" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId24" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId25">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId24" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1042" r:id="rId26" name="_ActiveXWrapper9">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1042" r:id="rId26" name="_ActiveXWrapper9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1043" r:id="rId28" name="_ActiveXWrapper10">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId29">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1043" r:id="rId28" name="_ActiveXWrapper10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1044" r:id="rId30" name="_ActiveXWrapper11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -10939,332 +11264,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1044" r:id="rId4" name="_ActiveXWrapper11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1043" r:id="rId6" name="_ActiveXWrapper10">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1043" r:id="rId6" name="_ActiveXWrapper10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId8" name="_ActiveXWrapper9">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1042" r:id="rId8" name="_ActiveXWrapper9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId10" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId10" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId12" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>161925</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1035" r:id="rId12" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>1048575</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId16" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>1048575</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1037" r:id="rId16" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId18" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1038" r:id="rId18" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId20" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1039" r:id="rId20" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1040" r:id="rId22" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1040" r:id="rId22" name="_ActiveXWrapper7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId24" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1041" r:id="rId24" name="_ActiveXWrapper8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1045" r:id="rId26" name="_ActiveXWrapper12">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>14</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>371475</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1045" r:id="rId26" name="_ActiveXWrapper12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1046" r:id="rId28" name="_ActiveXWrapper13">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId29">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1046" r:id="rId28" name="_ActiveXWrapper13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1047" r:id="rId30" name="_ActiveXWrapper14">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1047" r:id="rId30" name="_ActiveXWrapper14"/>
+        <control shapeId="1044" r:id="rId30" name="_ActiveXWrapper11"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11448,8 +11448,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="95237" r:id="rId4" name="_ActiveXWrapper4">
+        <control shapeId="95233" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>523875</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>285750</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="95233" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="95234" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>419100</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="95234" r:id="rId6" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="95235" r:id="rId8" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>504825</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="95235" r:id="rId8" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="95237" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
@@ -11468,82 +11543,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="95237" r:id="rId4" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="95235" r:id="rId6" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>504825</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="95235" r:id="rId6" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="95234" r:id="rId8" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>419100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="95234" r:id="rId8" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="95233" r:id="rId10" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>523875</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>285750</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="95233" r:id="rId10" name="_ActiveXWrapper1"/>
+        <control shapeId="95237" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11714,52 +11714,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37892" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="37896" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1019175</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>876300</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>714375</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37892" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="37896" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37893" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
+        <control shapeId="37895" r:id="rId6" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>771525</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>685800</xdr:colOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37893" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="37895" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11789,52 +11789,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37895" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+        <control shapeId="37893" r:id="rId10" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>771525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>685800</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37895" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="37893" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37896" r:id="rId12" name="_ActiveXWrapper5">
+        <control shapeId="37892" r:id="rId12" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>876300</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1019175</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>714375</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>123825</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37896" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="37892" r:id="rId12" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11995,8 +11995,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="28679" r:id="rId4" name="_ActiveXWrapper11">
+        <control shapeId="28678" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>266700</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28678" r:id="rId4" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28677" r:id="rId6" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28677" r:id="rId6" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28676" r:id="rId8" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28676" r:id="rId8" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28679" r:id="rId10" name="_ActiveXWrapper11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -12015,82 +12090,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="28679" r:id="rId4" name="_ActiveXWrapper11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28676" r:id="rId6" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>142875</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28676" r:id="rId6" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28677" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28677" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28678" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28678" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="28679" r:id="rId10" name="_ActiveXWrapper11"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12165,8 +12165,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="10241" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="10244" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1219200</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>990600</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10244" r:id="rId4" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10243" r:id="rId6" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1323975</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1095375</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10243" r:id="rId6" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10242" r:id="rId8" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1181100</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10242" r:id="rId8" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10241" r:id="rId10" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -12185,82 +12260,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="10241" r:id="rId4" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10242" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1181100</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10242" r:id="rId6" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10243" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1323975</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1095375</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10243" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10244" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1219200</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>990600</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10244" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="10241" r:id="rId10" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12475,8 +12475,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="81925" r:id="rId4" name="_ActiveXWrapper4">
+        <control shapeId="81927" r:id="rId4" name="_ActiveXWrapper6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>590550</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>590550</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81927" r:id="rId4" name="_ActiveXWrapper6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81926" r:id="rId6" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>161925</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81926" r:id="rId6" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81921" r:id="rId8" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1371600</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81921" r:id="rId8" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81922" r:id="rId10" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>104775</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81922" r:id="rId10" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81923" r:id="rId12" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81923" r:id="rId12" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81925" r:id="rId14" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>8</xdr:col>
@@ -12495,132 +12620,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="81925" r:id="rId4" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81923" r:id="rId6" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81923" r:id="rId6" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81922" r:id="rId8" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>104775</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81922" r:id="rId8" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81921" r:id="rId10" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>1371600</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81921" r:id="rId10" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81926" r:id="rId12" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>161925</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81926" r:id="rId12" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81927" r:id="rId14" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>590550</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>590550</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81927" r:id="rId14" name="_ActiveXWrapper6"/>
+        <control shapeId="81925" r:id="rId14" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12698,52 +12698,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4097" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="4101" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1381125</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1228725</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1152525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4097" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="4101" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4098" r:id="rId6" name="_ActiveXWrapper2">
+        <control shapeId="4100" r:id="rId6" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4098" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="4100" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12773,52 +12773,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4100" r:id="rId10" name="_ActiveXWrapper4">
+        <control shapeId="4098" r:id="rId10" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4100" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="4098" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4101" r:id="rId12" name="_ActiveXWrapper5">
+        <control shapeId="4097" r:id="rId12" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1381125</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1152525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1228725</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4101" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="4097" r:id="rId12" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13023,8 +13023,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="59401" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59401" r:id="rId4" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId6" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>485775</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>695325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId6" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId8" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>800100</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId8" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId10" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -13043,82 +13118,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59398" r:id="rId4" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>800100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId6" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>695325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59401" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="59398" r:id="rId10" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fix login form view
</commit_message>
<xml_diff>
--- a/DotNetExcel/StarkBankExcel/StarkBank.xlsx
+++ b/DotNetExcel/StarkBankExcel/StarkBank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stark - Admin\Documents\deploy-cartshop-hoje\sdk-excel\DotNetExcel\StarkBankExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4E8090-0C65-4706-9C73-C0318A3D2E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A16AF0-BCBA-43FE-A029-141FE825ED44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="1" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
   </bookViews>
@@ -399,7 +399,7 @@
     <t>Ex: 20018-183</t>
   </si>
   <si>
-    <t>Stark Bank SDK Excel - v3.1.1</t>
+    <t>Stark Bank SDK Excel - v3.1.2</t>
   </si>
 </sst>
 </file>
@@ -668,7 +668,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="23A4525A1295E524FB7284BA2EA2DC8317EF42"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="28A34ED1D2633F2429D291182761C070389522"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -685,7 +685,24 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="17053D61D1F15A1482019B2C1A4E6D57E3A971"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1626B229C1652514446181B314A00A77AF6681"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1F70BF05619C7F14D001A2031EA2288CEEF621"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -697,29 +714,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19A5453E610F18142DA1BAA91D29A587ED2E11"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4313"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D58F8DCE161321493A19D8C10118F3363B411"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="23FDAD7A329F60245422A56B22EA1482F84402"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -736,7 +736,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="10F831FB013D30140151820D1AB0BB140FD961"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2EF132486228D8243F428A6C298561D10E6622"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -753,7 +753,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="28A34ED1D2633F2429D291182761C070389522"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="23A4525A1295E524FB7284BA2EA2DC8317EF42"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -770,19 +770,36 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="15BA0FB321DE6D148D81BF60113447A8E50371"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5974E136658C5454320585C85BAB48B9439E65"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="397AE3E0A32833341B5399FC391E12926F72C3"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -799,36 +816,19 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="397AE3E0A32833341B5399FC391E12926F72C3"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="15BA0FB321DE6D148D81BF60113447A8E50371"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5974E136658C5454320585C85BAB48B9439E65"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -838,14 +838,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="80815DC5B82C3B8498489E26894C5C52875E28"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="43935BDA7439194471449D234CFD527D9886B4"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1588"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -855,7 +855,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2EF132486228D8243F428A6C298561D10E6622"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="10F831FB013D30140151820D1AB0BB140FD961"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -872,14 +872,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="71F4FF3617034374D487A4537B51302A0C89B7"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5FE4E9EDE5117D54C395AB0B52D849B4179075"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -906,14 +906,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5FE4E9EDE5117D54C395AB0B52D849B4179075"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="71F4FF3617034374D487A4537B51302A0C89B7"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -923,19 +923,70 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="43935BDA7439194471449D234CFD527D9886B4"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="80815DC5B82C3B8498489E26894C5C52875E28"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1588"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="75E9B6F4C78CB974E3679B0970BD37E29B8E77"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4DD8155564BBBB442F449A794155F293DF1F94"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="576D85FB2525B8547055A14351ED593B73E215"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -952,29 +1003,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="576D85FB2525B8547055A14351ED593B73E215"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4DD8155564BBBB442F449A794155F293DF1F94"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="17FA434AF19D0F14BB3186971AC86AABFB7FD1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -986,24 +1020,58 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX29.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="75E9B6F4C78CB974E3679B0970BD37E29B8E77"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="21156A5D42671D24110290D22610E26CEF0122"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D58F8DCE161321493A19D8C10118F3363B411"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX30.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="36BF4D76D36CAA346A9392633D35C8E7F4F293"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX31.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1020,75 +1088,92 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX32.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="36BF4D76D36CAA346A9392633D35C8E7F4F293"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="544CE9B5B5F4C8548335AFF35313355602FAD5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="23FDAD7A329F60245422A56B22EA1482F84402"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3AA2985733B4083434D3B3DA395B83B5AB5FB3"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="21156A5D42671D24110290D22610E26CEF0122"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="29E4B6D5F2B5EF24B732AC612476A095FC12F2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="17FA434AF19D0F14BB3186971AC86AABFB7FD1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1BF3F766D1EC8E14D641AB8818D8695A960D41"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6EAFFE9C06D4276431A6BB2F6072D3CF2C1786"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1105,97 +1190,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6EAFFE9C06D4276431A6BB2F6072D3CF2C1786"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1BF3F766D1EC8E14D641AB8818D8695A960D41"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="29E4B6D5F2B5EF24B732AC612476A095FC12F2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3AA2985733B4083434D3B3DA395B83B5AB5FB3"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="544CE9B5B5F4C8548335AFF35313355602FAD5"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX38.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5F3C3A5AA5DBB654AFD5A7C25896612CBE6DC5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D3C8440119274147F5190E81CB29314F1A0B1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1212,7 +1212,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4725C0A2E4AB894430D4AEF74EE21D1AD6A734"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2F27997732C2CB2441C298BB24A21C18565F42"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1229,13 +1229,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1F70BF05619C7F14D001A2031EA2288CEEF621"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19A5453E610F18142DA1BAA91D29A587ED2E11"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4313"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -1263,7 +1263,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2F27997732C2CB2441C298BB24A21C18565F42"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4725C0A2E4AB894430D4AEF74EE21D1AD6A734"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1280,7 +1280,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D3C8440119274147F5190E81CB29314F1A0B1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5F3C3A5AA5DBB654AFD5A7C25896612CBE6DC5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1297,19 +1297,36 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="9C5D0F81D9A7DC9451D986E29349E294E0E0F9"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6D5513A176D11B6489268BF06C26AC9C7986A6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX44.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="7B414461476FE874FCC7AF487111D4DE5C31F7"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX45.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1326,41 +1343,126 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX46.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="7B414461476FE874FCC7AF487111D4DE5C31F7"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="9C5D0F81D9A7DC9451D986E29349E294E0E0F9"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX47.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6D5513A176D11B6489268BF06C26AC9C7986A6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6DF62D0586063D64B576813E624CB2DFF23CB6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3334"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1217"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX48.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="581AFF66D5395E54CBC5BEBA52A895EF8D96F5"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX49.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4EDC5AE2D4725F442D54BDB348E5FBB86B52C4"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="17053D61D1F15A1482019B2C1A4E6D57E3A971"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3443F6D933A917348513994830A35447867593"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX51.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2F31A0EA52B80A243F02887A226A80BA2346A2"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3334"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1217"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX52.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1377,29 +1479,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX53.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2F31A0EA52B80A243F02887A226A80BA2346A2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3334"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1217"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX49.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3443F6D933A917348513994830A35447867593"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="55583C5835971E5409E5944455073F47DDC2A5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1411,29 +1496,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX54.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1626B229C1652514446181B314A00A77AF6681"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4EDC5AE2D4725F442D54BDB348E5FBB86B52C4"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="43443F65340DC5448034B84249A78BF6899C14"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1445,12 +1513,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX55.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="581AFF66D5395E54CBC5BEBA52A895EF8D96F5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="393B0D4DB376B1348C53AA283ED005A8E39383"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1462,24 +1530,41 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX56.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6DF62D0586063D64B576813E624CB2DFF23CB6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2FAFF23AA2246924D782B58F21CB01DE2B8C82"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3334"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1217"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX57.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="192AED9321906F1430518AA91C61F691A49AE1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX58.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1496,92 +1581,75 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX59.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="192AED9321906F1430518AA91C61F691A49AE1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="180E934D715B35148521A4DA16BAC3E49AA421"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2FAFF23AA2246924D782B58F21CB01DE2B8C82"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D1500907189BD14DA51B2181B162FBD75FE31"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX60.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="393B0D4DB376B1348C53AA283ED005A8E39383"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="209AD430929B0C246352BB46205966BBA32BE2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX61.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="43443F65340DC5448034B84249A78BF6899C14"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="340115F7C331F8342C23902032B2E1FE922923"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX58.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="55583C5835971E5409E5944455073F47DDC2A5"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX62.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -1598,80 +1666,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1DB344D2F14249140061BD5D11E614111405C1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4392"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX60.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="340115F7C331F8342C23902032B2E1FE922923"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX61.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="209AD430929B0C246352BB46205966BBA32BE2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX62.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="180E934D715B35148521A4DA16BAC3E49AA421"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX63.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5FCC13B9257A75548E65A9E458AA0E6A413BF5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1FF48C76A17A8C14A1D1B461189CB6BA129791"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1688,7 +1688,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4F2081B3648833443864BB8143FD2C02F9E634"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="23587ECD629DA1245032AC232F0D6B45106E92"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1722,7 +1722,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="23587ECD629DA1245032AC232F0D6B45106E92"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4F2081B3648833443864BB8143FD2C02F9E634"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1739,7 +1739,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1FF48C76A17A8C14A1D1B461189CB6BA129791"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5FCC13B9257A75548E65A9E458AA0E6A413BF5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1756,7 +1756,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19726D3BD1AD01142191B2C41B5B2D13E650B1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5B4A34D975B853543985A7E75523690B60EC35"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1773,7 +1773,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="207D2713820AB8246622A7CD26A57A9DCA2162"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="42576A9D548EA54490F4BA2045852D9EEA0264"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1790,14 +1790,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1CC3318201EE2A1421C19CEB15987574AED511"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1BD6BA4211BC3E14DAF185961A2B376D133421"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1824,7 +1824,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="42576A9D548EA54490F4BA2045852D9EEA0264"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="207D2713820AB8246622A7CD26A57A9DCA2162"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1841,7 +1841,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5B4A34D975B853543985A7E75523690B60EC35"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19726D3BD1AD01142191B2C41B5B2D13E650B1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1858,14 +1858,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="51A95A66553942547D759A7153A00908FCA885"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1B7A977A61ADF41453E1BBBE1183429619DB11"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3281"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1875,7 +1875,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4E23FE0EC4C93C4470948DA849AEEC73F9C744"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="232EEE2C927B21244D728DA228DC1AAB22C9E2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1909,7 +1909,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="232EEE2C927B21244D728DA228DC1AAB22C9E2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4E23FE0EC4C93C4470948DA849AEEC73F9C744"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1926,14 +1926,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1B7A977A61ADF41453E1BBBE1183429619DB11"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="51A95A66553942547D759A7153A00908FCA885"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3281"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1943,7 +1943,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="632A921A961CC6648D5697386AA1DF460A0236"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5B4126E875ABC55427F5B28E55218522354BA5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1960,13 +1960,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="245B62680258F8244B928BF02F0D73C394B3A2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="43953CE6E45013447B8491244183EC3B869614"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3149"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -1977,14 +1977,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1BD6BA4211BC3E14DAF185961A2B376D133421"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1CC3318201EE2A1421C19CEB15987574AED511"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2011,13 +2011,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="43953CE6E45013447B8491244183EC3B869614"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="245B62680258F8244B928BF02F0D73C394B3A2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3149"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -2028,7 +2028,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5B4126E875ABC55427F5B28E55218522354BA5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="632A921A961CC6648D5697386AA1DF460A0236"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2045,7 +2045,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="676BBF00A6812B64BBB6BA716DB953807A8EA6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="482B56B2D4F09144EA9495AD4E1391B3ADA544"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2062,7 +2062,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1441CBD291E7921466418469122C7CFF2CD931"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3C148BBC83328034CB4383F53575DFC2E2D673"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2096,7 +2096,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3C148BBC83328034CB4383F53575DFC2E2D673"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1441CBD291E7921466418469122C7CFF2CD931"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2113,7 +2113,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="482B56B2D4F09144EA9495AD4E1391B3ADA544"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="676BBF00A6812B64BBB6BA716DB953807A8EA6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2130,14 +2130,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1F6AA8BD81815014DA61A5D71870FA81614161"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="560AC6FB15F17754F6558A0F58035E0AF7ED85"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1482"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2147,7 +2147,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2596667A2285C4241122B3CF25CD7B218043C2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="423CD9C0343555445FB48C9D4CF7D65D1F3284"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2164,13 +2164,13 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D1500907189BD14DA51B2181B162FBD75FE31"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1DB344D2F14249140061BD5D11E614111405C1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4392"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -2198,7 +2198,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="423CD9C0343555445FB48C9D4CF7D65D1F3284"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2596667A2285C4241122B3CF25CD7B218043C2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2215,14 +2215,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="560AC6FB15F17754F6558A0F58035E0AF7ED85"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1F6AA8BD81815014DA61A5D71870FA81614161"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1482"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -8403,8 +8403,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3073" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="3078" r:id="rId4" name="_ActiveXWrapper6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>714375</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>485775</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3078" r:id="rId4" name="_ActiveXWrapper6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3077" r:id="rId6" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3077" r:id="rId6" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3076" r:id="rId8" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>723900</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3076" r:id="rId8" name="_ActiveXWrapper8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3075" r:id="rId10" name="_ActiveXWrapper7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3075" r:id="rId10" name="_ActiveXWrapper7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3074" r:id="rId12" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>561975</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3074" r:id="rId12" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3073" r:id="rId14" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
@@ -8423,132 +8548,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3073" r:id="rId4" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3074" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3074" r:id="rId6" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3075" r:id="rId8" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3075" r:id="rId8" name="_ActiveXWrapper7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3076" r:id="rId10" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>723900</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3076" r:id="rId10" name="_ActiveXWrapper8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3077" r:id="rId12" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3077" r:id="rId12" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3078" r:id="rId14" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>714375</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3078" r:id="rId14" name="_ActiveXWrapper6"/>
+        <control shapeId="3073" r:id="rId14" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8665,8 +8665,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="16390" r:id="rId4" name="_ActiveXWrapper6">
+        <control shapeId="16389" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1323975</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1095375</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16389" r:id="rId4" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16388" r:id="rId6" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1200150</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>971550</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16388" r:id="rId6" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16387" r:id="rId8" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1076325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16387" r:id="rId8" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16386" r:id="rId10" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1162050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16386" r:id="rId10" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16385" r:id="rId12" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1162050</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="16385" r:id="rId12" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="16390" r:id="rId14" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -8685,132 +8810,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="16390" r:id="rId4" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16385" r:id="rId6" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1162050</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16385" r:id="rId6" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16386" r:id="rId8" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1162050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16386" r:id="rId8" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16387" r:id="rId10" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1076325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16387" r:id="rId10" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16388" r:id="rId12" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>971550</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16388" r:id="rId12" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="16389" r:id="rId14" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1323975</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1095375</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="16389" r:id="rId14" name="_ActiveXWrapper5"/>
+        <control shapeId="16390" r:id="rId14" name="_ActiveXWrapper6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8917,8 +8917,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="73732" r:id="rId3" name="_ActiveXWrapper4">
+        <control shapeId="73729" r:id="rId3" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1314450</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>495300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="73729" r:id="rId3" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="73730" r:id="rId5" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>466725</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="73730" r:id="rId5" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="73731" r:id="rId7" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="73731" r:id="rId7" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="73732" r:id="rId9" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -8937,82 +9012,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="73732" r:id="rId3" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="73731" r:id="rId5" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="73731" r:id="rId5" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="73730" r:id="rId7" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>466725</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="73730" r:id="rId7" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="73729" r:id="rId9" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1314450</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>495300</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="73729" r:id="rId9" name="_ActiveXWrapper1"/>
+        <control shapeId="73732" r:id="rId9" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9158,52 +9158,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="52229" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="52225" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>1266825</xdr:colOff>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>180975</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>2428875</xdr:colOff>
+                <xdr:colOff>1181100</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="52229" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="52225" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="52228" r:id="rId6" name="_ActiveXWrapper4">
+        <control shapeId="52226" r:id="rId6" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>2514600</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>723900</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1171575</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="52228" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="52226" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9233,52 +9233,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="52226" r:id="rId10" name="_ActiveXWrapper2">
+        <control shapeId="52228" r:id="rId10" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>2514600</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1171575</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>723900</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="52226" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="52228" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="52225" r:id="rId12" name="_ActiveXWrapper1">
+        <control shapeId="52229" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>1266825</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>1181100</xdr:colOff>
+                <xdr:colOff>2428875</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="52225" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="52229" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9394,52 +9394,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20481" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="20485" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20481" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="20485" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20482" r:id="rId6" name="_ActiveXWrapper2">
+        <control shapeId="20484" r:id="rId6" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>390525</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20482" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="20484" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9469,52 +9469,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20484" r:id="rId10" name="_ActiveXWrapper4">
+        <control shapeId="20482" r:id="rId10" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>390525</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20484" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="20482" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20485" r:id="rId12" name="_ActiveXWrapper5">
+        <control shapeId="20481" r:id="rId12" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20485" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="20481" r:id="rId12" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9609,52 +9609,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8197" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="8193" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1257300</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8197" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="8193" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8196" r:id="rId6" name="_ActiveXWrapper4">
+        <control shapeId="8194" r:id="rId6" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1247775</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8196" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="8194" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9684,52 +9684,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8194" r:id="rId10" name="_ActiveXWrapper2">
+        <control shapeId="8196" r:id="rId10" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1247775</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8194" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="8196" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId12" name="_ActiveXWrapper1">
+        <control shapeId="8197" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1257300</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="8197" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9826,18 +9826,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="49158" r:id="rId4" name="_ActiveXWrapper10">
+        <control shapeId="49157" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>876300</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1485900</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>685800</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -9846,32 +9846,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="49158" r:id="rId4" name="_ActiveXWrapper10"/>
+        <control shapeId="49157" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="49154" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="49156" r:id="rId6" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1495425</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>942975</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>695325</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>2076450</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>95250</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="49154" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="49156" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9901,43 +9901,43 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="49156" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
+        <control shapeId="49154" r:id="rId10" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>942975</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1495425</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>2076450</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>695325</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="49156" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="49154" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="49157" r:id="rId12" name="_ActiveXWrapper5">
+        <control shapeId="49158" r:id="rId12" name="_ActiveXWrapper10">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1485900</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>876300</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>685800</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -9946,7 +9946,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="49157" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="49158" r:id="rId12" name="_ActiveXWrapper10"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10062,52 +10062,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24582" r:id="rId4" name="_ActiveXWrapper10">
+        <control shapeId="24580" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1209675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1123950</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>981075</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>895350</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24582" r:id="rId4" name="_ActiveXWrapper10"/>
+        <control shapeId="24580" r:id="rId4" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24577" r:id="rId6" name="_ActiveXWrapper1">
+        <control shapeId="24579" r:id="rId6" name="_ActiveXWrapper3">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1219200</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1047750</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>990600</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24577" r:id="rId6" name="_ActiveXWrapper1"/>
+        <control shapeId="24579" r:id="rId6" name="_ActiveXWrapper3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10137,52 +10137,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24579" r:id="rId10" name="_ActiveXWrapper3">
+        <control shapeId="24577" r:id="rId10" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1219200</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>990600</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1047750</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24579" r:id="rId10" name="_ActiveXWrapper3"/>
+        <control shapeId="24577" r:id="rId10" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24580" r:id="rId12" name="_ActiveXWrapper4">
+        <control shapeId="24582" r:id="rId12" name="_ActiveXWrapper10">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1123950</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1209675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>895350</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>981075</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24580" r:id="rId12" name="_ActiveXWrapper4"/>
+        <control shapeId="24582" r:id="rId12" name="_ActiveXWrapper10"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10267,52 +10267,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6145" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="6149" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>1333500</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>47625</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1152525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1114425</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6145" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="6149" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6146" r:id="rId6" name="_ActiveXWrapper2">
+        <control shapeId="6148" r:id="rId6" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1247775</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1171575</xdr:colOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>1028700</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>123825</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6146" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="6148" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10342,52 +10342,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6148" r:id="rId10" name="_ActiveXWrapper4">
+        <control shapeId="6146" r:id="rId10" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>1247775</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>1028700</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1171575</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6148" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="6146" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6149" r:id="rId12" name="_ActiveXWrapper5">
+        <control shapeId="6145" r:id="rId12" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>1333500</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>47625</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>1114425</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1152525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6149" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="6145" r:id="rId12" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10400,7 +10400,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:M10"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -10919,8 +10919,333 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1047" r:id="rId4" name="_ActiveXWrapper14">
+        <control shapeId="1044" r:id="rId4" name="_ActiveXWrapper11">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>514350</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1044" r:id="rId4" name="_ActiveXWrapper11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1043" r:id="rId6" name="_ActiveXWrapper10">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1043" r:id="rId6" name="_ActiveXWrapper10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1042" r:id="rId8" name="_ActiveXWrapper9">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1042" r:id="rId8" name="_ActiveXWrapper9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId10" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId10" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId12" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>161925</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1035" r:id="rId12" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>266700</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>1048575</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1037" r:id="rId16" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>1048575</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1037" r:id="rId16" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1038" r:id="rId18" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId18" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1039" r:id="rId20" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1039" r:id="rId20" name="_ActiveXWrapper6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1040" r:id="rId22" name="_ActiveXWrapper7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1040" r:id="rId22" name="_ActiveXWrapper7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1041" r:id="rId24" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1041" r:id="rId24" name="_ActiveXWrapper8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1045" r:id="rId26" name="_ActiveXWrapper12">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>14</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>371475</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1045" r:id="rId26" name="_ActiveXWrapper12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1046" r:id="rId28" name="_ActiveXWrapper13">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId29">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>19</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1046" r:id="rId28" name="_ActiveXWrapper13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1047" r:id="rId30" name="_ActiveXWrapper14">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>16</xdr:col>
@@ -10939,332 +11264,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1047" r:id="rId4" name="_ActiveXWrapper14"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1046" r:id="rId6" name="_ActiveXWrapper13">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1046" r:id="rId6" name="_ActiveXWrapper13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1045" r:id="rId8" name="_ActiveXWrapper12">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>14</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>371475</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1045" r:id="rId8" name="_ActiveXWrapper12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId10" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1041" r:id="rId10" name="_ActiveXWrapper8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1040" r:id="rId12" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1040" r:id="rId12" name="_ActiveXWrapper7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId14" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1039" r:id="rId14" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId16" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1038" r:id="rId16" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId18" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>1048575</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1037" r:id="rId18" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId20" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>1048575</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1036" r:id="rId20" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId22" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>161925</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1035" r:id="rId22" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId24" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId25">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId24" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId26" name="_ActiveXWrapper9">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1042" r:id="rId26" name="_ActiveXWrapper9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1043" r:id="rId28" name="_ActiveXWrapper10">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId29">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1043" r:id="rId28" name="_ActiveXWrapper10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1044" r:id="rId30" name="_ActiveXWrapper11">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>142875</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1044" r:id="rId30" name="_ActiveXWrapper11"/>
+        <control shapeId="1047" r:id="rId30" name="_ActiveXWrapper14"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11448,8 +11448,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="95233" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="95237" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>752475</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="95237" r:id="rId4" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="95235" r:id="rId6" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>504825</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="95235" r:id="rId6" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="95234" r:id="rId8" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>419100</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="95234" r:id="rId8" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="95233" r:id="rId10" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -11468,82 +11543,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="95233" r:id="rId4" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="95234" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>419100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="95234" r:id="rId6" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="95235" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>504825</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="95235" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="95237" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>752475</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="95237" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="95233" r:id="rId10" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11714,52 +11714,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37896" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="37892" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>876300</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1019175</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>714375</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>123825</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37896" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="37892" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37895" r:id="rId6" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="37893" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>771525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>685800</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37895" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="37893" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11789,52 +11789,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37893" r:id="rId10" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
+        <control shapeId="37895" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>771525</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>685800</xdr:colOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37893" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="37895" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37892" r:id="rId12" name="_ActiveXWrapper1">
+        <control shapeId="37896" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1019175</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>876300</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>714375</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37892" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="37896" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11995,8 +11995,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="28678" r:id="rId4" name="_ActiveXWrapper4">
+        <control shapeId="28679" r:id="rId4" name="_ActiveXWrapper11">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>285750</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>161925</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28679" r:id="rId4" name="_ActiveXWrapper11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28676" r:id="rId6" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28676" r:id="rId6" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28677" r:id="rId8" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28677" r:id="rId8" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28678" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -12015,82 +12090,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="28678" r:id="rId4" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28677" r:id="rId6" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28677" r:id="rId6" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28676" r:id="rId8" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>142875</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28676" r:id="rId8" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28679" r:id="rId10" name="_ActiveXWrapper11">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>285750</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>161925</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28679" r:id="rId10" name="_ActiveXWrapper11"/>
+        <control shapeId="28678" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12165,8 +12165,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="10244" r:id="rId4" name="_ActiveXWrapper4">
+        <control shapeId="10241" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1181100</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10241" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10242" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1181100</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10242" r:id="rId6" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10243" r:id="rId8" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1323975</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1095375</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10243" r:id="rId8" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10244" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
@@ -12185,82 +12260,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="10244" r:id="rId4" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10243" r:id="rId6" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1323975</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1095375</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10243" r:id="rId6" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10242" r:id="rId8" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1181100</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10242" r:id="rId8" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10241" r:id="rId10" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1181100</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10241" r:id="rId10" name="_ActiveXWrapper1"/>
+        <control shapeId="10244" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12475,8 +12475,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="81927" r:id="rId4" name="_ActiveXWrapper6">
+        <control shapeId="81925" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>628650</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81925" r:id="rId4" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81923" r:id="rId6" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81923" r:id="rId6" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81922" r:id="rId8" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>104775</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81922" r:id="rId8" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81921" r:id="rId10" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1371600</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81921" r:id="rId10" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81926" r:id="rId12" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>161925</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="81926" r:id="rId12" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="81927" r:id="rId14" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>8</xdr:col>
@@ -12495,132 +12620,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="81927" r:id="rId4" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81926" r:id="rId6" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>161925</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81926" r:id="rId6" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81921" r:id="rId8" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>1371600</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81921" r:id="rId8" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81922" r:id="rId10" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>104775</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81922" r:id="rId10" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81923" r:id="rId12" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81923" r:id="rId12" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="81925" r:id="rId14" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>628650</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="81925" r:id="rId14" name="_ActiveXWrapper4"/>
+        <control shapeId="81927" r:id="rId14" name="_ActiveXWrapper6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12698,52 +12698,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4101" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="4097" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1381125</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1152525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1228725</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4101" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="4097" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4100" r:id="rId6" name="_ActiveXWrapper4">
+        <control shapeId="4098" r:id="rId6" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4100" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="4098" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12773,52 +12773,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4098" r:id="rId10" name="_ActiveXWrapper2">
+        <control shapeId="4100" r:id="rId10" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4098" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="4100" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4097" r:id="rId12" name="_ActiveXWrapper1">
+        <control shapeId="4101" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1381125</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1228725</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1152525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4097" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="4101" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13023,8 +13023,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId4" name="_ActiveXWrapper4">
+        <control shapeId="59398" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>495300</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>657225</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>800100</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId6" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId8" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>485775</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>695325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId8" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59401" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>7</xdr:col>
@@ -13043,82 +13118,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59401" r:id="rId4" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId6" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>695325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId6" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId8" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>800100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId8" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId10" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>495300</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>657225</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId10" name="_ActiveXWrapper1"/>
+        <control shapeId="59401" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fix paymentRequest, boletoPayment, login, corporatePurchase issues
</commit_message>
<xml_diff>
--- a/DotNetExcel/StarkBankExcel/StarkBank.xlsx
+++ b/DotNetExcel/StarkBankExcel/StarkBank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stark - Admin\Documents\deploy-cartshop-hoje\sdk-excel\DotNetExcel\StarkBankExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E8F73F-50A1-43A6-BFC6-FDE8BEFB3377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245EA1CE-57CE-4C7B-A933-319AB7860723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="1" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="1" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="2" state="hidden" r:id="rId1"/>
@@ -428,7 +428,7 @@
     <t>Split 3</t>
   </si>
   <si>
-    <t>Stark Bank SDK Excel - v3.1.4</t>
+    <t>Stark Bank SDK Excel - v3.1.5</t>
   </si>
 </sst>
 </file>
@@ -9103,7 +9103,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9160,6 +9160,11 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H1048576" xr:uid="{451E9477-2BA9-49AF-BA0F-B0B2A54F2877}">
+      <formula1>"checking, savings, salary, payment"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -11475,7 +11480,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -13850,7 +13855,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add tags to boleto
</commit_message>
<xml_diff>
--- a/DotNetExcel/StarkBankExcel/StarkBank.xlsx
+++ b/DotNetExcel/StarkBankExcel/StarkBank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stark - Admin\Documents\deploy-cartshop-hoje\sdk-excel\DotNetExcel\StarkBankExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DD8512-0D12-4D35-8655-5A62AB0CCB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1463D52D-777A-4492-9529-907ADD610B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="1" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7785" firstSheet="13" activeTab="14" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="2" state="hidden" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="122">
   <si>
     <t>Chave Pix</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Juro ao Mês</t>
   </si>
   <si>
-    <t>Dias para Baixa Automática</t>
-  </si>
-  <si>
     <t>Olá</t>
   </si>
   <si>
@@ -431,7 +428,7 @@
     <t>Nome do CardHolder</t>
   </si>
   <si>
-    <t>Stark Bank SDK Excel - v3.2.1</t>
+    <t>Stark Bank SDK Excel - v3.3.0</t>
   </si>
 </sst>
 </file>
@@ -9149,7 +9146,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>9</v>
@@ -9452,10 +9449,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>87</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>3</v>
@@ -9464,13 +9461,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H9" s="29" t="s">
         <v>2</v>
@@ -9479,10 +9476,10 @@
         <v>4</v>
       </c>
       <c r="J9" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>7</v>
@@ -9855,7 +9852,7 @@
     <row r="5" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E6" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -9898,7 +9895,7 @@
         <v>56</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>32</v>
@@ -10168,13 +10165,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="C9" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>3</v>
@@ -10297,9 +10294,9 @@
   <sheetPr codeName="Planilha14"/>
   <dimension ref="A1:XFC9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10398,7 +10395,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>1</v>
@@ -10407,7 +10404,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>59</v>
@@ -10419,7 +10416,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -10876,16 +10873,16 @@
         <v>33</v>
       </c>
       <c r="Q9" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="R9" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="S9" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="S9" s="14" t="s">
+      <c r="T9" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -11093,16 +11090,16 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -11248,7 +11245,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11312,8 +11309,8 @@
       <c r="L9" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="M9" s="12" t="s">
-        <v>64</v>
+      <c r="M9" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>17</v>
@@ -11334,12 +11331,14 @@
         <v>22</v>
       </c>
       <c r="T9" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U9" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="V9" s="21"/>
+        <v>100</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -11482,8 +11481,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -11494,7 +11493,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -11518,7 +11517,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -11722,7 +11721,7 @@
       <c r="L10" s="37"/>
       <c r="M10" s="37"/>
       <c r="N10" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O10" s="37"/>
       <c r="P10" s="37"/>
@@ -11799,7 +11798,7 @@
     </row>
     <row r="14" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="37"/>
       <c r="C14" s="37"/>
@@ -12689,22 +12688,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>106</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>107</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>49</v>
@@ -12716,7 +12715,7 @@
         <v>51</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>53</v>
@@ -12724,14 +12723,14 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="33"/>
       <c r="E10" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="33" t="s">
         <v>110</v>
-      </c>
-      <c r="K10" s="33" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -12939,10 +12938,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>5</v>
@@ -13191,7 +13190,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>7</v>
@@ -13200,10 +13199,10 @@
         <v>8</v>
       </c>
       <c r="F9" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -13445,16 +13444,16 @@
         <v>43</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>72</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>24</v>
@@ -13463,13 +13462,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="J9" s="20" t="s">
         <v>74</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -13732,10 +13731,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>3</v>
@@ -13744,10 +13743,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9" s="20" t="s">
         <v>2</v>
@@ -14191,10 +14190,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>1</v>
@@ -14209,28 +14208,28 @@
         <v>5</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>7</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>9</v>
       </c>
       <c r="K9" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="L9" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="M9" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="N9" s="32" t="s">
         <v>99</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>